<commit_message>
Updated entry files for Wall bracing window development
</commit_message>
<xml_diff>
--- a/Scripts/SeizmikaPodaci.xlsx
+++ b/Scripts/SeizmikaPodaci.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikolal\Documents\Git\grf-bg\BetonskeKonstrukcije\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikolal\Documents\Git\CivEngine\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4168CBCB-823F-43C1-9A6F-033D77BF2E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC166D33-E030-4E5C-8D9D-06FB32708129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3610" yWindow="2970" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Naziv platna</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Razmak pridrzanih sipki bi [cm]</t>
+  </si>
+  <si>
+    <t>b500b</t>
+  </si>
+  <si>
+    <t>ABP A2</t>
   </si>
 </sst>
 </file>
@@ -390,21 +396,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="9" max="9" width="7.36328125" customWidth="1"/>
+    <col min="10" max="10" width="19.54296875" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" customWidth="1"/>
+    <col min="13" max="13" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,6 +453,63 @@
       </c>
       <c r="M1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1622</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>180</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>45</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <f>144 + 56</f>
+        <v>200</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M5">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added excel file for input for scripts including seismic calculation
</commit_message>
<xml_diff>
--- a/Scripts/SeizmikaPodaci.xlsx
+++ b/Scripts/SeizmikaPodaci.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikolal\Documents\Git\grf-bg\BetonskeKonstrukcije\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlaki\Documents\Git\CivEngine\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4168CBCB-823F-43C1-9A6F-033D77BF2E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBA4DFA-FA04-4D99-9841-6A92CD06EDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -393,18 +393,25 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" customWidth="1"/>
+    <col min="9" max="9" width="33.1796875" customWidth="1"/>
+    <col min="10" max="10" width="23.36328125" customWidth="1"/>
+    <col min="11" max="11" width="28.26953125" customWidth="1"/>
+    <col min="13" max="13" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>